<commit_message>
Profils et php mailer
</commit_message>
<xml_diff>
--- a/documentations/Gantt site LPRS.xlsx
+++ b/documentations/Gantt site LPRS.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1CF1964-58CE-49A9-883C-C381DC30FED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{C4445231-6056-4BA6-8385-F6A2FA0971CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECF02E1B-4CC4-4CC3-A28C-9A8019DE1279}"/>
   <bookViews>
-    <workbookView xWindow="2748" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PlanningProjet" sheetId="11" r:id="rId1"/>
@@ -1466,9 +1466,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="57" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="168" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -1478,14 +1475,17 @@
     <xf numFmtId="168" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8">
       <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="8" applyBorder="1">
       <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="3" xfId="9">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -2337,15 +2337,15 @@
   </sheetPr>
   <dimension ref="A1:EE51"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="69" zoomScaleNormal="15" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B25" sqref="B25"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScale="54" zoomScaleNormal="15" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.6640625" style="38" customWidth="1"/>
-    <col min="2" max="2" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="30.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.109375" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
@@ -2395,207 +2395,207 @@
       <c r="B3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="102" t="s">
+      <c r="C3" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="103"/>
-      <c r="E3" s="101">
+      <c r="D3" s="101"/>
+      <c r="E3" s="102">
         <f ca="1">TODAY()</f>
-        <v>45572</v>
-      </c>
-      <c r="F3" s="101"/>
+        <v>45551</v>
+      </c>
+      <c r="F3" s="102"/>
     </row>
     <row r="4" spans="1:135" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="102" t="s">
+      <c r="C4" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="103"/>
+      <c r="D4" s="101"/>
       <c r="E4" s="6">
         <v>1</v>
       </c>
-      <c r="I4" s="98">
+      <c r="I4" s="97">
         <f ca="1">I5</f>
+        <v>45551</v>
+      </c>
+      <c r="J4" s="98"/>
+      <c r="K4" s="98"/>
+      <c r="L4" s="98"/>
+      <c r="M4" s="98"/>
+      <c r="N4" s="98"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="97">
+        <f ca="1">P5</f>
+        <v>45558</v>
+      </c>
+      <c r="Q4" s="98"/>
+      <c r="R4" s="98"/>
+      <c r="S4" s="98"/>
+      <c r="T4" s="98"/>
+      <c r="U4" s="98"/>
+      <c r="V4" s="99"/>
+      <c r="W4" s="97">
+        <f ca="1">W5</f>
+        <v>45565</v>
+      </c>
+      <c r="X4" s="98"/>
+      <c r="Y4" s="98"/>
+      <c r="Z4" s="98"/>
+      <c r="AA4" s="98"/>
+      <c r="AB4" s="98"/>
+      <c r="AC4" s="99"/>
+      <c r="AD4" s="97">
+        <f ca="1">AD5</f>
         <v>45572</v>
       </c>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="99"/>
-      <c r="N4" s="99"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="98">
-        <f ca="1">P5</f>
+      <c r="AE4" s="98"/>
+      <c r="AF4" s="98"/>
+      <c r="AG4" s="98"/>
+      <c r="AH4" s="98"/>
+      <c r="AI4" s="98"/>
+      <c r="AJ4" s="99"/>
+      <c r="AK4" s="97">
+        <f ca="1">AK5</f>
         <v>45579</v>
       </c>
-      <c r="Q4" s="99"/>
-      <c r="R4" s="99"/>
-      <c r="S4" s="99"/>
-      <c r="T4" s="99"/>
-      <c r="U4" s="99"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="98">
-        <f ca="1">W5</f>
+      <c r="AL4" s="98"/>
+      <c r="AM4" s="98"/>
+      <c r="AN4" s="98"/>
+      <c r="AO4" s="98"/>
+      <c r="AP4" s="98"/>
+      <c r="AQ4" s="99"/>
+      <c r="AR4" s="97">
+        <f ca="1">AR5</f>
         <v>45586</v>
       </c>
-      <c r="X4" s="99"/>
-      <c r="Y4" s="99"/>
-      <c r="Z4" s="99"/>
-      <c r="AA4" s="99"/>
-      <c r="AB4" s="99"/>
-      <c r="AC4" s="100"/>
-      <c r="AD4" s="98">
-        <f ca="1">AD5</f>
+      <c r="AS4" s="98"/>
+      <c r="AT4" s="98"/>
+      <c r="AU4" s="98"/>
+      <c r="AV4" s="98"/>
+      <c r="AW4" s="98"/>
+      <c r="AX4" s="99"/>
+      <c r="AY4" s="97">
+        <f ca="1">AY5</f>
         <v>45593</v>
       </c>
-      <c r="AE4" s="99"/>
-      <c r="AF4" s="99"/>
-      <c r="AG4" s="99"/>
-      <c r="AH4" s="99"/>
-      <c r="AI4" s="99"/>
-      <c r="AJ4" s="100"/>
-      <c r="AK4" s="98">
-        <f ca="1">AK5</f>
+      <c r="AZ4" s="98"/>
+      <c r="BA4" s="98"/>
+      <c r="BB4" s="98"/>
+      <c r="BC4" s="98"/>
+      <c r="BD4" s="98"/>
+      <c r="BE4" s="99"/>
+      <c r="BF4" s="97">
+        <f ca="1">BF5</f>
         <v>45600</v>
       </c>
-      <c r="AL4" s="99"/>
-      <c r="AM4" s="99"/>
-      <c r="AN4" s="99"/>
-      <c r="AO4" s="99"/>
-      <c r="AP4" s="99"/>
-      <c r="AQ4" s="100"/>
-      <c r="AR4" s="98">
-        <f ca="1">AR5</f>
+      <c r="BG4" s="98"/>
+      <c r="BH4" s="98"/>
+      <c r="BI4" s="98"/>
+      <c r="BJ4" s="98"/>
+      <c r="BK4" s="98"/>
+      <c r="BL4" s="99"/>
+      <c r="BM4" s="97">
+        <f ca="1">BM5</f>
         <v>45607</v>
       </c>
-      <c r="AS4" s="99"/>
-      <c r="AT4" s="99"/>
-      <c r="AU4" s="99"/>
-      <c r="AV4" s="99"/>
-      <c r="AW4" s="99"/>
-      <c r="AX4" s="100"/>
-      <c r="AY4" s="98">
-        <f ca="1">AY5</f>
+      <c r="BN4" s="98"/>
+      <c r="BO4" s="98"/>
+      <c r="BP4" s="98"/>
+      <c r="BQ4" s="98"/>
+      <c r="BR4" s="98"/>
+      <c r="BS4" s="99"/>
+      <c r="BT4" s="97">
+        <f t="shared" ref="BT4" ca="1" si="0">BT5</f>
         <v>45614</v>
       </c>
-      <c r="AZ4" s="99"/>
-      <c r="BA4" s="99"/>
-      <c r="BB4" s="99"/>
-      <c r="BC4" s="99"/>
-      <c r="BD4" s="99"/>
-      <c r="BE4" s="100"/>
-      <c r="BF4" s="98">
-        <f ca="1">BF5</f>
+      <c r="BU4" s="98"/>
+      <c r="BV4" s="98"/>
+      <c r="BW4" s="98"/>
+      <c r="BX4" s="98"/>
+      <c r="BY4" s="98"/>
+      <c r="BZ4" s="99"/>
+      <c r="CA4" s="97">
+        <f t="shared" ref="CA4" ca="1" si="1">CA5</f>
         <v>45621</v>
       </c>
-      <c r="BG4" s="99"/>
-      <c r="BH4" s="99"/>
-      <c r="BI4" s="99"/>
-      <c r="BJ4" s="99"/>
-      <c r="BK4" s="99"/>
-      <c r="BL4" s="100"/>
-      <c r="BM4" s="98">
-        <f ca="1">BM5</f>
+      <c r="CB4" s="98"/>
+      <c r="CC4" s="98"/>
+      <c r="CD4" s="98"/>
+      <c r="CE4" s="98"/>
+      <c r="CF4" s="98"/>
+      <c r="CG4" s="99"/>
+      <c r="CH4" s="97">
+        <f t="shared" ref="CH4" ca="1" si="2">CH5</f>
         <v>45628</v>
       </c>
-      <c r="BN4" s="99"/>
-      <c r="BO4" s="99"/>
-      <c r="BP4" s="99"/>
-      <c r="BQ4" s="99"/>
-      <c r="BR4" s="99"/>
-      <c r="BS4" s="100"/>
-      <c r="BT4" s="98">
-        <f t="shared" ref="BT4" ca="1" si="0">BT5</f>
+      <c r="CI4" s="98"/>
+      <c r="CJ4" s="98"/>
+      <c r="CK4" s="98"/>
+      <c r="CL4" s="98"/>
+      <c r="CM4" s="98"/>
+      <c r="CN4" s="99"/>
+      <c r="CO4" s="97">
+        <f t="shared" ref="CO4" ca="1" si="3">CO5</f>
         <v>45635</v>
       </c>
-      <c r="BU4" s="99"/>
-      <c r="BV4" s="99"/>
-      <c r="BW4" s="99"/>
-      <c r="BX4" s="99"/>
-      <c r="BY4" s="99"/>
-      <c r="BZ4" s="100"/>
-      <c r="CA4" s="98">
-        <f t="shared" ref="CA4" ca="1" si="1">CA5</f>
+      <c r="CP4" s="98"/>
+      <c r="CQ4" s="98"/>
+      <c r="CR4" s="98"/>
+      <c r="CS4" s="98"/>
+      <c r="CT4" s="98"/>
+      <c r="CU4" s="99"/>
+      <c r="CV4" s="97">
+        <f t="shared" ref="CV4" ca="1" si="4">CV5</f>
         <v>45642</v>
       </c>
-      <c r="CB4" s="99"/>
-      <c r="CC4" s="99"/>
-      <c r="CD4" s="99"/>
-      <c r="CE4" s="99"/>
-      <c r="CF4" s="99"/>
-      <c r="CG4" s="100"/>
-      <c r="CH4" s="98">
-        <f t="shared" ref="CH4" ca="1" si="2">CH5</f>
+      <c r="CW4" s="98"/>
+      <c r="CX4" s="98"/>
+      <c r="CY4" s="98"/>
+      <c r="CZ4" s="98"/>
+      <c r="DA4" s="98"/>
+      <c r="DB4" s="99"/>
+      <c r="DC4" s="97">
+        <f t="shared" ref="DC4" ca="1" si="5">DC5</f>
         <v>45649</v>
       </c>
-      <c r="CI4" s="99"/>
-      <c r="CJ4" s="99"/>
-      <c r="CK4" s="99"/>
-      <c r="CL4" s="99"/>
-      <c r="CM4" s="99"/>
-      <c r="CN4" s="100"/>
-      <c r="CO4" s="98">
-        <f t="shared" ref="CO4" ca="1" si="3">CO5</f>
+      <c r="DD4" s="98"/>
+      <c r="DE4" s="98"/>
+      <c r="DF4" s="98"/>
+      <c r="DG4" s="98"/>
+      <c r="DH4" s="98"/>
+      <c r="DI4" s="99"/>
+      <c r="DJ4" s="97">
+        <f t="shared" ref="DJ4" ca="1" si="6">DJ5</f>
         <v>45656</v>
       </c>
-      <c r="CP4" s="99"/>
-      <c r="CQ4" s="99"/>
-      <c r="CR4" s="99"/>
-      <c r="CS4" s="99"/>
-      <c r="CT4" s="99"/>
-      <c r="CU4" s="100"/>
-      <c r="CV4" s="98">
-        <f t="shared" ref="CV4" ca="1" si="4">CV5</f>
+      <c r="DK4" s="98"/>
+      <c r="DL4" s="98"/>
+      <c r="DM4" s="98"/>
+      <c r="DN4" s="98"/>
+      <c r="DO4" s="98"/>
+      <c r="DP4" s="99"/>
+      <c r="DQ4" s="97">
+        <f t="shared" ref="DQ4" ca="1" si="7">DQ5</f>
         <v>45663</v>
       </c>
-      <c r="CW4" s="99"/>
-      <c r="CX4" s="99"/>
-      <c r="CY4" s="99"/>
-      <c r="CZ4" s="99"/>
-      <c r="DA4" s="99"/>
-      <c r="DB4" s="100"/>
-      <c r="DC4" s="98">
-        <f t="shared" ref="DC4" ca="1" si="5">DC5</f>
+      <c r="DR4" s="98"/>
+      <c r="DS4" s="98"/>
+      <c r="DT4" s="98"/>
+      <c r="DU4" s="98"/>
+      <c r="DV4" s="98"/>
+      <c r="DW4" s="99"/>
+      <c r="DX4" s="97">
+        <f t="shared" ref="DX4" ca="1" si="8">DX5</f>
         <v>45670</v>
       </c>
-      <c r="DD4" s="99"/>
-      <c r="DE4" s="99"/>
-      <c r="DF4" s="99"/>
-      <c r="DG4" s="99"/>
-      <c r="DH4" s="99"/>
-      <c r="DI4" s="100"/>
-      <c r="DJ4" s="98">
-        <f t="shared" ref="DJ4" ca="1" si="6">DJ5</f>
-        <v>45677</v>
-      </c>
-      <c r="DK4" s="99"/>
-      <c r="DL4" s="99"/>
-      <c r="DM4" s="99"/>
-      <c r="DN4" s="99"/>
-      <c r="DO4" s="99"/>
-      <c r="DP4" s="100"/>
-      <c r="DQ4" s="98">
-        <f t="shared" ref="DQ4" ca="1" si="7">DQ5</f>
-        <v>45684</v>
-      </c>
-      <c r="DR4" s="99"/>
-      <c r="DS4" s="99"/>
-      <c r="DT4" s="99"/>
-      <c r="DU4" s="99"/>
-      <c r="DV4" s="99"/>
-      <c r="DW4" s="100"/>
-      <c r="DX4" s="98">
-        <f t="shared" ref="DX4" ca="1" si="8">DX5</f>
-        <v>45691</v>
-      </c>
-      <c r="DY4" s="99"/>
-      <c r="DZ4" s="99"/>
-      <c r="EA4" s="99"/>
-      <c r="EB4" s="99"/>
-      <c r="EC4" s="99"/>
-      <c r="ED4" s="100"/>
+      <c r="DY4" s="98"/>
+      <c r="DZ4" s="98"/>
+      <c r="EA4" s="98"/>
+      <c r="EB4" s="98"/>
+      <c r="EC4" s="98"/>
+      <c r="ED4" s="99"/>
     </row>
     <row r="5" spans="1:135" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="39" t="s">
@@ -2609,507 +2609,507 @@
       <c r="G5" s="56"/>
       <c r="I5" s="72">
         <f ca="1">Début_Projet-WEEKDAY(Début_Projet,1)+2+7*(Semaine_Affichage-1)</f>
-        <v>45572</v>
+        <v>45551</v>
       </c>
       <c r="J5" s="73">
         <f ca="1">I5+1</f>
-        <v>45573</v>
+        <v>45552</v>
       </c>
       <c r="K5" s="73">
         <f t="shared" ref="K5:AX5" ca="1" si="9">J5+1</f>
-        <v>45574</v>
+        <v>45553</v>
       </c>
       <c r="L5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45575</v>
+        <v>45554</v>
       </c>
       <c r="M5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45576</v>
+        <v>45555</v>
       </c>
       <c r="N5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45577</v>
+        <v>45556</v>
       </c>
       <c r="O5" s="74">
         <f t="shared" ca="1" si="9"/>
-        <v>45578</v>
+        <v>45557</v>
       </c>
       <c r="P5" s="72">
         <f ca="1">O5+1</f>
-        <v>45579</v>
+        <v>45558</v>
       </c>
       <c r="Q5" s="73">
         <f ca="1">P5+1</f>
-        <v>45580</v>
+        <v>45559</v>
       </c>
       <c r="R5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45581</v>
+        <v>45560</v>
       </c>
       <c r="S5" s="73">
         <f t="shared" ref="S5" ca="1" si="10">R5+1</f>
-        <v>45582</v>
+        <v>45561</v>
       </c>
       <c r="T5" s="73">
         <f t="shared" ref="T5" ca="1" si="11">S5+1</f>
-        <v>45583</v>
+        <v>45562</v>
       </c>
       <c r="U5" s="73">
         <f t="shared" ref="U5" ca="1" si="12">T5+1</f>
-        <v>45584</v>
+        <v>45563</v>
       </c>
       <c r="V5" s="73">
         <f t="shared" ref="V5" ca="1" si="13">U5+1</f>
-        <v>45585</v>
+        <v>45564</v>
       </c>
       <c r="W5" s="73">
         <f t="shared" ref="W5" ca="1" si="14">V5+1</f>
-        <v>45586</v>
+        <v>45565</v>
       </c>
       <c r="X5" s="73">
         <f t="shared" ref="X5" ca="1" si="15">W5+1</f>
-        <v>45587</v>
+        <v>45566</v>
       </c>
       <c r="Y5" s="73">
         <f t="shared" ref="Y5" ca="1" si="16">X5+1</f>
-        <v>45588</v>
+        <v>45567</v>
       </c>
       <c r="Z5" s="73">
         <f t="shared" ref="Z5" ca="1" si="17">Y5+1</f>
-        <v>45589</v>
+        <v>45568</v>
       </c>
       <c r="AA5" s="73">
         <f t="shared" ref="AA5" ca="1" si="18">Z5+1</f>
-        <v>45590</v>
+        <v>45569</v>
       </c>
       <c r="AB5" s="73">
         <f t="shared" ref="AB5" ca="1" si="19">AA5+1</f>
-        <v>45591</v>
+        <v>45570</v>
       </c>
       <c r="AC5" s="73">
         <f t="shared" ref="AC5" ca="1" si="20">AB5+1</f>
-        <v>45592</v>
+        <v>45571</v>
       </c>
       <c r="AD5" s="73">
         <f t="shared" ref="AD5" ca="1" si="21">AC5+1</f>
-        <v>45593</v>
+        <v>45572</v>
       </c>
       <c r="AE5" s="73">
         <f t="shared" ref="AE5" ca="1" si="22">AD5+1</f>
-        <v>45594</v>
+        <v>45573</v>
       </c>
       <c r="AF5" s="73">
         <f t="shared" ref="AF5" ca="1" si="23">AE5+1</f>
-        <v>45595</v>
+        <v>45574</v>
       </c>
       <c r="AG5" s="73">
         <f t="shared" ref="AG5" ca="1" si="24">AF5+1</f>
-        <v>45596</v>
+        <v>45575</v>
       </c>
       <c r="AH5" s="73">
         <f t="shared" ref="AH5" ca="1" si="25">AG5+1</f>
-        <v>45597</v>
+        <v>45576</v>
       </c>
       <c r="AI5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45598</v>
+        <v>45577</v>
       </c>
       <c r="AJ5" s="74">
         <f t="shared" ca="1" si="9"/>
-        <v>45599</v>
+        <v>45578</v>
       </c>
       <c r="AK5" s="72">
         <f ca="1">AJ5+1</f>
-        <v>45600</v>
+        <v>45579</v>
       </c>
       <c r="AL5" s="73">
         <f ca="1">AK5+1</f>
-        <v>45601</v>
+        <v>45580</v>
       </c>
       <c r="AM5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45602</v>
+        <v>45581</v>
       </c>
       <c r="AN5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45603</v>
+        <v>45582</v>
       </c>
       <c r="AO5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45604</v>
+        <v>45583</v>
       </c>
       <c r="AP5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45605</v>
+        <v>45584</v>
       </c>
       <c r="AQ5" s="74">
         <f t="shared" ca="1" si="9"/>
-        <v>45606</v>
+        <v>45585</v>
       </c>
       <c r="AR5" s="72">
         <f ca="1">AQ5+1</f>
-        <v>45607</v>
+        <v>45586</v>
       </c>
       <c r="AS5" s="73">
         <f ca="1">AR5+1</f>
-        <v>45608</v>
+        <v>45587</v>
       </c>
       <c r="AT5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45609</v>
+        <v>45588</v>
       </c>
       <c r="AU5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45610</v>
+        <v>45589</v>
       </c>
       <c r="AV5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45611</v>
+        <v>45590</v>
       </c>
       <c r="AW5" s="73">
         <f t="shared" ca="1" si="9"/>
-        <v>45612</v>
+        <v>45591</v>
       </c>
       <c r="AX5" s="74">
         <f t="shared" ca="1" si="9"/>
-        <v>45613</v>
+        <v>45592</v>
       </c>
       <c r="AY5" s="72">
         <f ca="1">AX5+1</f>
-        <v>45614</v>
+        <v>45593</v>
       </c>
       <c r="AZ5" s="73">
         <f ca="1">AY5+1</f>
-        <v>45615</v>
+        <v>45594</v>
       </c>
       <c r="BA5" s="73">
         <f t="shared" ref="BA5:BE5" ca="1" si="26">AZ5+1</f>
-        <v>45616</v>
+        <v>45595</v>
       </c>
       <c r="BB5" s="73">
         <f t="shared" ca="1" si="26"/>
-        <v>45617</v>
+        <v>45596</v>
       </c>
       <c r="BC5" s="73">
         <f t="shared" ca="1" si="26"/>
-        <v>45618</v>
+        <v>45597</v>
       </c>
       <c r="BD5" s="73">
         <f t="shared" ca="1" si="26"/>
-        <v>45619</v>
+        <v>45598</v>
       </c>
       <c r="BE5" s="74">
         <f t="shared" ca="1" si="26"/>
-        <v>45620</v>
+        <v>45599</v>
       </c>
       <c r="BF5" s="72">
         <f ca="1">BE5+1</f>
-        <v>45621</v>
+        <v>45600</v>
       </c>
       <c r="BG5" s="73">
         <f ca="1">BF5+1</f>
-        <v>45622</v>
+        <v>45601</v>
       </c>
       <c r="BH5" s="73">
         <f t="shared" ref="BH5:BK5" ca="1" si="27">BG5+1</f>
-        <v>45623</v>
+        <v>45602</v>
       </c>
       <c r="BI5" s="73">
         <f t="shared" ca="1" si="27"/>
-        <v>45624</v>
+        <v>45603</v>
       </c>
       <c r="BJ5" s="73">
         <f t="shared" ca="1" si="27"/>
-        <v>45625</v>
+        <v>45604</v>
       </c>
       <c r="BK5" s="73">
         <f t="shared" ca="1" si="27"/>
-        <v>45626</v>
+        <v>45605</v>
       </c>
       <c r="BL5" s="74">
         <f ca="1">BK5+1</f>
-        <v>45627</v>
+        <v>45606</v>
       </c>
       <c r="BM5" s="74">
         <f t="shared" ref="BM5:DX5" ca="1" si="28">BL5+1</f>
-        <v>45628</v>
+        <v>45607</v>
       </c>
       <c r="BN5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45629</v>
+        <v>45608</v>
       </c>
       <c r="BO5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45630</v>
+        <v>45609</v>
       </c>
       <c r="BP5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45631</v>
+        <v>45610</v>
       </c>
       <c r="BQ5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45632</v>
+        <v>45611</v>
       </c>
       <c r="BR5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45633</v>
+        <v>45612</v>
       </c>
       <c r="BS5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45634</v>
+        <v>45613</v>
       </c>
       <c r="BT5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45635</v>
+        <v>45614</v>
       </c>
       <c r="BU5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45636</v>
+        <v>45615</v>
       </c>
       <c r="BV5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45637</v>
+        <v>45616</v>
       </c>
       <c r="BW5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45638</v>
+        <v>45617</v>
       </c>
       <c r="BX5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45639</v>
+        <v>45618</v>
       </c>
       <c r="BY5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45640</v>
+        <v>45619</v>
       </c>
       <c r="BZ5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45641</v>
+        <v>45620</v>
       </c>
       <c r="CA5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45642</v>
+        <v>45621</v>
       </c>
       <c r="CB5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45643</v>
+        <v>45622</v>
       </c>
       <c r="CC5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45644</v>
+        <v>45623</v>
       </c>
       <c r="CD5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45645</v>
+        <v>45624</v>
       </c>
       <c r="CE5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45646</v>
+        <v>45625</v>
       </c>
       <c r="CF5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45647</v>
+        <v>45626</v>
       </c>
       <c r="CG5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45648</v>
+        <v>45627</v>
       </c>
       <c r="CH5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45649</v>
+        <v>45628</v>
       </c>
       <c r="CI5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45650</v>
+        <v>45629</v>
       </c>
       <c r="CJ5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45651</v>
+        <v>45630</v>
       </c>
       <c r="CK5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45652</v>
+        <v>45631</v>
       </c>
       <c r="CL5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45653</v>
+        <v>45632</v>
       </c>
       <c r="CM5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45654</v>
+        <v>45633</v>
       </c>
       <c r="CN5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45655</v>
+        <v>45634</v>
       </c>
       <c r="CO5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45656</v>
+        <v>45635</v>
       </c>
       <c r="CP5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45657</v>
+        <v>45636</v>
       </c>
       <c r="CQ5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45658</v>
+        <v>45637</v>
       </c>
       <c r="CR5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45659</v>
+        <v>45638</v>
       </c>
       <c r="CS5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45660</v>
+        <v>45639</v>
       </c>
       <c r="CT5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45661</v>
+        <v>45640</v>
       </c>
       <c r="CU5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45662</v>
+        <v>45641</v>
       </c>
       <c r="CV5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45663</v>
+        <v>45642</v>
       </c>
       <c r="CW5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45664</v>
+        <v>45643</v>
       </c>
       <c r="CX5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45665</v>
+        <v>45644</v>
       </c>
       <c r="CY5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45666</v>
+        <v>45645</v>
       </c>
       <c r="CZ5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45667</v>
+        <v>45646</v>
       </c>
       <c r="DA5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45668</v>
+        <v>45647</v>
       </c>
       <c r="DB5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45669</v>
+        <v>45648</v>
       </c>
       <c r="DC5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45670</v>
+        <v>45649</v>
       </c>
       <c r="DD5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45671</v>
+        <v>45650</v>
       </c>
       <c r="DE5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45672</v>
+        <v>45651</v>
       </c>
       <c r="DF5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45673</v>
+        <v>45652</v>
       </c>
       <c r="DG5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45674</v>
+        <v>45653</v>
       </c>
       <c r="DH5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45675</v>
+        <v>45654</v>
       </c>
       <c r="DI5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45676</v>
+        <v>45655</v>
       </c>
       <c r="DJ5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45677</v>
+        <v>45656</v>
       </c>
       <c r="DK5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45678</v>
+        <v>45657</v>
       </c>
       <c r="DL5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45679</v>
+        <v>45658</v>
       </c>
       <c r="DM5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45680</v>
+        <v>45659</v>
       </c>
       <c r="DN5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45681</v>
+        <v>45660</v>
       </c>
       <c r="DO5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45682</v>
+        <v>45661</v>
       </c>
       <c r="DP5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45683</v>
+        <v>45662</v>
       </c>
       <c r="DQ5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45684</v>
+        <v>45663</v>
       </c>
       <c r="DR5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45685</v>
+        <v>45664</v>
       </c>
       <c r="DS5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45686</v>
+        <v>45665</v>
       </c>
       <c r="DT5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45687</v>
+        <v>45666</v>
       </c>
       <c r="DU5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45688</v>
+        <v>45667</v>
       </c>
       <c r="DV5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45689</v>
+        <v>45668</v>
       </c>
       <c r="DW5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45690</v>
+        <v>45669</v>
       </c>
       <c r="DX5" s="74">
         <f t="shared" ca="1" si="28"/>
-        <v>45691</v>
+        <v>45670</v>
       </c>
       <c r="DY5" s="74">
         <f t="shared" ref="DY5:ED5" ca="1" si="29">DX5+1</f>
-        <v>45692</v>
+        <v>45671</v>
       </c>
       <c r="DZ5" s="74">
         <f t="shared" ca="1" si="29"/>
-        <v>45693</v>
+        <v>45672</v>
       </c>
       <c r="EA5" s="74">
         <f t="shared" ca="1" si="29"/>
-        <v>45694</v>
+        <v>45673</v>
       </c>
       <c r="EB5" s="74">
         <f t="shared" ca="1" si="29"/>
-        <v>45695</v>
+        <v>45674</v>
       </c>
       <c r="EC5" s="74">
         <f t="shared" ca="1" si="29"/>
-        <v>45696</v>
+        <v>45675</v>
       </c>
       <c r="ED5" s="74">
         <f t="shared" ca="1" si="29"/>
-        <v>45697</v>
+        <v>45676</v>
       </c>
       <c r="EE5" s="74"/>
     </row>
@@ -3866,11 +3866,11 @@
       </c>
       <c r="E9" s="62">
         <f ca="1">Début_Projet</f>
-        <v>45572</v>
+        <v>45551</v>
       </c>
       <c r="F9" s="62">
         <f ca="1">E9+3</f>
-        <v>45575</v>
+        <v>45554</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10">
@@ -3881,7 +3881,7 @@
       <c r="J9" s="75"/>
       <c r="K9" s="75"/>
       <c r="L9" s="75"/>
-      <c r="M9" s="97"/>
+      <c r="M9" s="103"/>
       <c r="N9" s="24"/>
       <c r="O9" s="24"/>
       <c r="P9" s="24"/>
@@ -4019,11 +4019,11 @@
       </c>
       <c r="E10" s="62">
         <f ca="1">F9</f>
-        <v>45575</v>
+        <v>45554</v>
       </c>
       <c r="F10" s="62">
         <f ca="1">E10+2</f>
-        <v>45577</v>
+        <v>45556</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
@@ -4167,11 +4167,11 @@
       </c>
       <c r="E11" s="62">
         <f ca="1">F10</f>
-        <v>45577</v>
+        <v>45556</v>
       </c>
       <c r="F11" s="62">
         <f ca="1">E11+4</f>
-        <v>45581</v>
+        <v>45560</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10">
@@ -4316,11 +4316,11 @@
       </c>
       <c r="E12" s="62">
         <f ca="1">F11</f>
-        <v>45581</v>
+        <v>45560</v>
       </c>
       <c r="F12" s="62">
         <f ca="1">E12+5</f>
-        <v>45586</v>
+        <v>45565</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10">
@@ -4464,11 +4464,11 @@
       <c r="D13" s="13"/>
       <c r="E13" s="62">
         <f ca="1">E10+1</f>
-        <v>45576</v>
+        <v>45555</v>
       </c>
       <c r="F13" s="62">
         <f ca="1">E13+2</f>
-        <v>45578</v>
+        <v>45557</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10">
@@ -4750,11 +4750,11 @@
       </c>
       <c r="E15" s="65">
         <f ca="1">E13+1</f>
-        <v>45577</v>
+        <v>45556</v>
       </c>
       <c r="F15" s="65">
         <f ca="1">E15+4</f>
-        <v>45581</v>
+        <v>45560</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="10">
@@ -4896,11 +4896,11 @@
       </c>
       <c r="E16" s="65">
         <f ca="1">E15+2</f>
-        <v>45579</v>
+        <v>45558</v>
       </c>
       <c r="F16" s="65">
         <f ca="1">E16+5</f>
-        <v>45584</v>
+        <v>45563</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10">
@@ -5045,11 +5045,11 @@
       <c r="D17" s="16"/>
       <c r="E17" s="65">
         <f ca="1">F16</f>
-        <v>45584</v>
+        <v>45563</v>
       </c>
       <c r="F17" s="65">
         <f ca="1">E17+3</f>
-        <v>45587</v>
+        <v>45566</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10">
@@ -5192,11 +5192,11 @@
       <c r="D18" s="16"/>
       <c r="E18" s="65">
         <f ca="1">E17</f>
-        <v>45584</v>
+        <v>45563</v>
       </c>
       <c r="F18" s="65">
         <f ca="1">E18+2</f>
-        <v>45586</v>
+        <v>45565</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="10">
@@ -5340,11 +5340,11 @@
       <c r="D19" s="16"/>
       <c r="E19" s="65">
         <f ca="1">E18</f>
-        <v>45584</v>
+        <v>45563</v>
       </c>
       <c r="F19" s="65">
         <f ca="1">E19+3</f>
-        <v>45587</v>
+        <v>45566</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10">
@@ -5632,11 +5632,11 @@
       <c r="D21" s="19"/>
       <c r="E21" s="68">
         <f ca="1">E9+15</f>
-        <v>45587</v>
+        <v>45566</v>
       </c>
       <c r="F21" s="68">
         <f ca="1">E21+5</f>
-        <v>45592</v>
+        <v>45571</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="10">
@@ -5774,11 +5774,11 @@
       <c r="D22" s="19"/>
       <c r="E22" s="68">
         <f ca="1">F21+1</f>
-        <v>45593</v>
+        <v>45572</v>
       </c>
       <c r="F22" s="68">
         <f ca="1">E22+4</f>
-        <v>45597</v>
+        <v>45576</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="10">
@@ -5923,11 +5923,11 @@
       <c r="D23" s="19"/>
       <c r="E23" s="68">
         <f ca="1">E22+5</f>
-        <v>45598</v>
+        <v>45577</v>
       </c>
       <c r="F23" s="68">
         <f ca="1">E23+5</f>
-        <v>45603</v>
+        <v>45582</v>
       </c>
       <c r="G23" s="10"/>
       <c r="H23" s="10">
@@ -6068,11 +6068,11 @@
       <c r="D24" s="19"/>
       <c r="E24" s="68">
         <f ca="1">F23+1</f>
-        <v>45604</v>
+        <v>45583</v>
       </c>
       <c r="F24" s="68">
         <f ca="1">E24+4</f>
-        <v>45608</v>
+        <v>45587</v>
       </c>
       <c r="G24" s="10"/>
       <c r="H24" s="10">
@@ -6206,7 +6206,7 @@
       <c r="EC24" s="24"/>
       <c r="ED24" s="24"/>
     </row>
-    <row r="25" spans="1:134" s="3" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:134" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="38"/>
       <c r="B25" s="54" t="s">
         <v>51</v>
@@ -6217,11 +6217,11 @@
       <c r="D25" s="19"/>
       <c r="E25" s="68">
         <f ca="1">E23</f>
-        <v>45598</v>
+        <v>45577</v>
       </c>
       <c r="F25" s="68">
         <f ca="1">E25+4</f>
-        <v>45602</v>
+        <v>45581</v>
       </c>
       <c r="G25" s="10"/>
       <c r="H25" s="10">
@@ -9972,27 +9972,27 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="CV4:DB4"/>
-    <mergeCell ref="DC4:DI4"/>
-    <mergeCell ref="DJ4:DP4"/>
-    <mergeCell ref="DQ4:DW4"/>
-    <mergeCell ref="DX4:ED4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="CO4:CU4"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="CO4:CU4"/>
+    <mergeCell ref="CV4:DB4"/>
+    <mergeCell ref="DC4:DI4"/>
+    <mergeCell ref="DJ4:DP4"/>
+    <mergeCell ref="DQ4:DW4"/>
+    <mergeCell ref="DX4:ED4"/>
   </mergeCells>
   <phoneticPr fontId="33" type="noConversion"/>
   <conditionalFormatting sqref="D7:D31">
@@ -10009,104 +10009,104 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:BL8 BM8:ED8 I9:BK9 BL9:ED31 O10:BK10 P11 U11:BK11 I11:M12 O12:T12 X12:BK12 I13:L13 U13:V13 AB13:BK13 I14:BK14 I15:M15 S15:V15 Z15:BK15 I16:O16 V16:BK16 Y17:AJ17 AP17:AV17 AX17:BK17 I17:T19 X18:AJ18 AL18:BK18 Y19:BK19 I20:BK20 I21:U21 AD21:BK21 I22:AB22 AI22:BK22 I23:AH23 AP23:BK23 I24:AM24 AT24:BK24 I25:AG25 AN25:BK25 I26:BK36 BL32:BU32 BW32:ED32 BL33:ED36 BM5:EE5 BM6:ED6">
-    <cfRule type="expression" dxfId="26" priority="33">
+  <conditionalFormatting sqref="I5:BL8 BM8:ED8 O10:BK10 P11 U11:BK11 I11:M12 O12:T12 X12:BK12 I13:L13 U13:V13 AB13:BK13 I14:BK14 I15:M15 S15:V15 Z15:BK15 I16:O16 V16:BK16 Y17:AJ17 AP17:AV17 AX17:BK17 I17:T19 X18:AJ18 AL18:BK18 Y19:BK19 I20:BK20 I21:U21 AD21:BK21 I22:AB22 AI22:BK22 I23:AH23 AP23:BK23 I24:AM24 AT24:BK24 I25:AG25 AN25:BK25 I26:BK36 BL32:BU32 BW32:ED32 BL33:ED36 BM5:EE5 BM6:ED6 I9:BK9 BL9:ED31">
+    <cfRule type="expression" dxfId="2" priority="33">
       <formula>AND(TODAY()&gt;=I$5,TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I7:BL8 BM8:ED8 I9:BK9 BL9:ED31 O10:BK10 P11 U11:BK11 I11:M12 O12:T12 X12:BK12 I13:L13 U13:V13 AB13:BK13 I14:BK14 I15:M15 S15:V15 Z15:BK15 I16:O16 V16:BK16 Y17:AJ17 AP17:AV17 AX17:BK17 I17:T19 X18:AJ18 AL18:BK18 Y19:BK19 I20:BK20 I21:U21 AD21:BK21 I22:AB22 AI22:BK22 I23:AH23 AP23:BK23 I24:AM24 AT24:BK24 I25:AG25 AN25:BK25 I26:BK36 BL32:BU32 BW32:ED32 BL33:ED36">
-    <cfRule type="expression" dxfId="25" priority="27">
+  <conditionalFormatting sqref="I7:BL8 BM8:ED8 O10:BK10 P11 U11:BK11 I11:M12 O12:T12 X12:BK12 I13:L13 U13:V13 AB13:BK13 I14:BK14 I15:M15 S15:V15 Z15:BK15 I16:O16 V16:BK16 Y17:AJ17 AP17:AV17 AX17:BK17 I17:T19 X18:AJ18 AL18:BK18 Y19:BK19 I20:BK20 I21:U21 AD21:BK21 I22:AB22 AI22:BK22 I23:AH23 AP23:BK23 I24:AM24 AT24:BK24 I25:AG25 AN25:BK25 I26:BK36 BL32:BU32 BW32:ED32 BL33:ED36 I9:BK9 BL9:ED31">
+    <cfRule type="expression" dxfId="1" priority="27">
       <formula>AND(début_tâche&lt;=I$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="28" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=I$5,début_tâche&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P10">
-    <cfRule type="expression" dxfId="23" priority="35">
+    <cfRule type="expression" dxfId="26" priority="35">
       <formula>AND(TODAY()&gt;=M$5,TODAY()&lt;N$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="38">
+    <cfRule type="expression" dxfId="25" priority="38">
       <formula>AND(début_tâche&lt;=M$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=M$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="39" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=M$5,début_tâche&lt;N$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P12">
-    <cfRule type="expression" dxfId="20" priority="53">
+    <cfRule type="expression" dxfId="23" priority="53">
       <formula>AND(TODAY()&gt;=R$5,TODAY()&lt;S$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="56">
+    <cfRule type="expression" dxfId="22" priority="56">
       <formula>AND(début_tâche&lt;=R$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=R$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="57" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=R$5,début_tâche&lt;S$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q10">
-    <cfRule type="expression" dxfId="17" priority="41">
+    <cfRule type="expression" dxfId="20" priority="41">
       <formula>AND(TODAY()&gt;=L$5,TODAY()&lt;M$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="44">
+    <cfRule type="expression" dxfId="19" priority="44">
       <formula>AND(début_tâche&lt;=L$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=L$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="45" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="45" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=L$5,début_tâche&lt;M$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R10">
-    <cfRule type="expression" dxfId="14" priority="47">
+    <cfRule type="expression" dxfId="17" priority="47">
       <formula>AND(TODAY()&gt;=K$5,TODAY()&lt;L$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="50">
+    <cfRule type="expression" dxfId="16" priority="50">
       <formula>AND(début_tâche&lt;=K$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=K$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="51" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="51" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=K$5,début_tâche&lt;L$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W13:AA13 BV32">
-    <cfRule type="expression" dxfId="11" priority="95">
+    <cfRule type="expression" dxfId="14" priority="95">
       <formula>AND(TODAY()&gt;=X$5,TODAY()&lt;Y$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="98">
+    <cfRule type="expression" dxfId="13" priority="98">
       <formula>AND(début_tâche&lt;=X$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=X$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="99" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="99" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=X$5,début_tâche&lt;Y$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD15:AH15">
-    <cfRule type="expression" dxfId="8" priority="100">
+    <cfRule type="expression" dxfId="11" priority="100">
       <formula>AND(TODAY()&gt;=R$5,TODAY()&lt;S$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="101">
+    <cfRule type="expression" dxfId="10" priority="101">
       <formula>AND(début_tâche&lt;=R$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=R$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="102" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="102" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=R$5,début_tâche&lt;S$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL17:AO17">
-    <cfRule type="expression" dxfId="5" priority="83">
+    <cfRule type="expression" dxfId="8" priority="83">
       <formula>AND(TODAY()&gt;=Y$5,TODAY()&lt;Z$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="86">
+    <cfRule type="expression" dxfId="7" priority="86">
       <formula>AND(début_tâche&lt;=Y$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=Y$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="87" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="87" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=Y$5,début_tâche&lt;Z$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR17:AV17">
-    <cfRule type="expression" dxfId="2" priority="89">
+    <cfRule type="expression" dxfId="5" priority="89">
       <formula>AND(TODAY()&gt;=AB$5,TODAY()&lt;AC$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="92">
+    <cfRule type="expression" dxfId="4" priority="92">
       <formula>AND(début_tâche&lt;=AB$5,ROUNDDOWN((fin_tâche-début_tâche+1)*avancement_tâche,0)+début_tâche-1&gt;=AB$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="93" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="93" stopIfTrue="1">
       <formula>AND(fin_tâche&gt;=AB$5,début_tâche&lt;AC$5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10262,23 +10262,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="0d3ed9b3-bd2a-4d91-a92e-f5a0b1862000" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC6FC1DE444E8C419AC02378D2CA4A97" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="d23fc6208c54a75e43afb64f8786bd7c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0d3ed9b3-bd2a-4d91-a92e-f5a0b1862000" xmlns:ns4="fed57df8-ef22-47fe-89ca-65918babccf6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1b6cb9cbd86112f0ca357c573d2defd" ns3:_="" ns4:_="">
     <xsd:import namespace="0d3ed9b3-bd2a-4d91-a92e-f5a0b1862000"/>
@@ -10505,10 +10488,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="0d3ed9b3-bd2a-4d91-a92e-f5a0b1862000" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86DDC6D4-B1B0-4EB8-94CD-2A4EA753AC2F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0d3ed9b3-bd2a-4d91-a92e-f5a0b1862000"/>
+    <ds:schemaRef ds:uri="fed57df8-ef22-47fe-89ca-65918babccf6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -10531,20 +10542,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86DDC6D4-B1B0-4EB8-94CD-2A4EA753AC2F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0d3ed9b3-bd2a-4d91-a92e-f5a0b1862000"/>
-    <ds:schemaRef ds:uri="fed57df8-ef22-47fe-89ca-65918babccf6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>